<commit_message>
adding AWA calculation improvements
</commit_message>
<xml_diff>
--- a/calc/static/calc/piql_prices.xlsx
+++ b/calc/static/calc/piql_prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\PycharmProjects\calculator\calc\static\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037456C5-AD53-41A9-815C-CAC4885772B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC6CDF4-CD3C-4C14-B082-1AF8ABFA062D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
   </bookViews>
@@ -365,9 +365,6 @@
     <t>awa_reel_pickup_fee</t>
   </si>
   <si>
-    <t>piqlReader_instalation</t>
-  </si>
-  <si>
     <t>piqlReader_platinum_service</t>
   </si>
   <si>
@@ -393,6 +390,9 @@
   </si>
   <si>
     <t>piqlConnect_monthly</t>
+  </si>
+  <si>
+    <t>piqlReader_installation</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD7F3CE-3398-4BFC-A88A-63EE7D330900}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.5"/>
@@ -790,7 +790,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
         <v>67</v>
@@ -799,7 +799,7 @@
         <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -832,7 +832,7 @@
         <v>521</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
@@ -843,7 +843,7 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
@@ -857,12 +857,12 @@
         <v>675</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7">
         <v>830</v>
@@ -885,7 +885,7 @@
         <v>236</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.5">
@@ -1238,7 +1238,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B38">
         <v>3000</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B39">
         <v>4000</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40">
         <v>2500</v>

</xml_diff>

<commit_message>
change the prices for online storage
</commit_message>
<xml_diff>
--- a/calc/static/calc/piql_prices.xlsx
+++ b/calc/static/calc/piql_prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\PycharmProjects\calculator\calc\static\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18E8FFE-A126-4F89-A859-C935EC0A69B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BFE7C3-0434-4F79-A08E-B9102903B0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="17770" tabRatio="781" xr2:uid="{D64C4359-5929-4BBC-9F5D-572B5F120BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="prices" sheetId="13" r:id="rId1"/>
@@ -782,7 +782,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.5"/>

</xml_diff>